<commit_message>
Added email body code for salesmen
</commit_message>
<xml_diff>
--- a/AdvisoryBoardTracking.xlsx
+++ b/AdvisoryBoardTracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John Paradise\MyPythonScripts\AdvisoryBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77304322-8E65-4887-B867-F3B9E2BDF6FE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C874E32C-5048-4D2D-BF97-A632954CEFF6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10988" activeTab="1" xr2:uid="{16EC1FD0-7CA3-47E8-B2E3-1D4E6D661775}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10988" xr2:uid="{16EC1FD0-7CA3-47E8-B2E3-1D4E6D661775}"/>
   </bookViews>
   <sheets>
     <sheet name="NewSubmissions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>SO#</t>
   </si>
@@ -85,15 +85,9 @@
     <t>Bigman</t>
   </si>
   <si>
-    <t>Kings County Hospital</t>
-  </si>
-  <si>
     <t>689 NY Ave</t>
   </si>
   <si>
-    <t>18A0194</t>
-  </si>
-  <si>
     <t>Unassigned</t>
   </si>
   <si>
@@ -137,6 +131,15 @@
   </si>
   <si>
     <t>Billy</t>
+  </si>
+  <si>
+    <t>Boobs</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>June</t>
   </si>
 </sst>
 </file>
@@ -491,10 +494,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EEE128-BC57-4ED5-B88C-215F6AB7547E}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -541,13 +544,13 @@
         <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N1" t="s">
         <v>9</v>
@@ -569,6 +572,9 @@
       <c r="E2" t="s">
         <v>14</v>
       </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
       <c r="I2" t="s">
         <v>15</v>
       </c>
@@ -592,20 +598,20 @@
       <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="J3" t="s">
         <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
       </c>
       <c r="K3" t="s">
         <v>17</v>
@@ -622,37 +628,37 @@
         <v>1507094</v>
       </c>
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
       <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="1">
-        <v>42948</v>
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="I4" t="s">
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N4">
         <v>54111</v>
@@ -668,7 +674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4336759-1B85-4BCB-B4FE-7D008B816532}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
     </sheetView>
@@ -705,13 +711,13 @@
         <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -719,10 +725,10 @@
         <v>1234546</v>
       </c>
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
         <v>31</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
       </c>
       <c r="D2">
         <v>1234</v>
@@ -731,10 +737,10 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
@@ -745,22 +751,22 @@
         <v>9876545</v>
       </c>
       <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
         <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>36</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to email body and added a submittal date loop to know when we need to submit by
</commit_message>
<xml_diff>
--- a/AdvisoryBoardTracking.xlsx
+++ b/AdvisoryBoardTracking.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john\Desktop\AdvisoryBoardStatusEmailer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F189560-37C5-4788-A4A6-62DB27B0A15A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22EB3DC-0783-4F94-9AEF-8CA404D22B93}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10995" xr2:uid="{16EC1FD0-7CA3-47E8-B2E3-1D4E6D661775}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10995" activeTab="2" xr2:uid="{16EC1FD0-7CA3-47E8-B2E3-1D4E6D661775}"/>
   </bookViews>
   <sheets>
     <sheet name="NewSubmissions" sheetId="1" r:id="rId1"/>
     <sheet name="PendingReSubmissions" sheetId="2" r:id="rId2"/>
+    <sheet name="MeetingSchedule" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NewSubmissions!$A$1:$N$1</definedName>
@@ -876,27 +877,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -905,9 +891,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -920,6 +903,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6830,1959 +6814,1947 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EEE128-BC57-4ED5-B88C-215F6AB7547E}">
   <dimension ref="A1:N80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="2"/>
-    <col min="11" max="11" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1507093</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="2">
-        <v>53611</v>
+      <c r="A2" s="1">
+        <v>1312171</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1710133</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>14</v>
+      <c r="A3" s="1">
+        <v>1411083</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="1">
+        <v>53934</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1704031</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="2">
-        <v>54558</v>
+      <c r="A4" s="1">
+        <v>1411184</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1024</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="1">
+        <v>53664</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>1701112</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="2">
-        <v>54418</v>
+      <c r="A5" s="1">
+        <v>1503101</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="1">
+        <v>53667</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>1611103</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="2">
-        <v>54365</v>
+      <c r="A6" s="1">
+        <v>1503201</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="1">
+        <v>53439</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>1510012</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" s="2">
-        <v>53438</v>
+      <c r="A7" s="1">
+        <v>1503201</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="1">
+        <v>53831</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>1610042</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N8" s="2">
-        <v>54348</v>
+      <c r="A8" s="1">
+        <v>1504271</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="1">
+        <v>54020</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>1610041</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="2">
-        <v>54351</v>
+      <c r="A9" s="1">
+        <v>1504282</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="1">
+        <v>53266</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>1510022</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N10" s="2">
-        <v>53370</v>
+      <c r="A10" s="1">
+        <v>1507061</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="1">
+        <v>53617</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>1606061</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N11" s="2">
-        <v>53976</v>
+      <c r="A11" s="1">
+        <v>1507093</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="1">
+        <v>53611</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>1607201</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N12" s="2">
-        <v>54087</v>
+      <c r="A12" s="1">
+        <v>1507094</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="1">
+        <v>54111</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>1701201</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N13" s="2">
-        <v>54416</v>
+      <c r="A13" s="1">
+        <v>1507142</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="1">
+        <v>53802</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>1603154</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N14" s="2">
-        <v>53641</v>
+      <c r="A14" s="1">
+        <v>1507284</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14" s="1">
+        <v>53275</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>1601074</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N15" s="2">
-        <v>53457</v>
+      <c r="A15" s="1">
+        <v>1510012</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N15" s="1">
+        <v>53438</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>1503201</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N16" s="2">
-        <v>53439</v>
+      <c r="A16" s="1">
+        <v>1510022</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N16" s="1">
+        <v>53370</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>1503201</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N17" s="2">
-        <v>53831</v>
+      <c r="A17" s="1">
+        <v>1510072</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" s="1">
+        <v>53335</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>1611085</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N18" s="2">
-        <v>54705</v>
+      <c r="A18" s="1">
+        <v>1510094</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N18" s="1">
+        <v>53525</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>1608303</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N19" s="2">
-        <v>54162</v>
+      <c r="A19" s="1">
+        <v>1510291</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N19" s="1">
+        <v>53337</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>1708141</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N20" s="2">
-        <v>54871</v>
+      <c r="A20" s="1">
+        <v>1511181</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N20" s="1">
+        <v>53609</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>1705111</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N21" s="2">
-        <v>54724</v>
+      <c r="A21" s="1">
+        <v>1512175</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N21" s="1">
+        <v>53422</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>1701057</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N22" s="2">
-        <v>54521</v>
+      <c r="A22" s="1">
+        <v>1512176</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N22" s="1">
+        <v>53656</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>1612271</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N23" s="2">
-        <v>54414</v>
+      <c r="A23" s="1">
+        <v>1512177</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N23" s="1">
+        <v>53425</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>1606164</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N24" s="2">
-        <v>54066</v>
+      <c r="A24" s="1">
+        <v>1512178</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N24" s="1">
+        <v>53415</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>1606164</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N25" s="2">
-        <v>54033</v>
+      <c r="A25" s="1">
+        <v>1512179</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N25" s="1">
+        <v>53416</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>1601284</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N26" s="2">
-        <v>53591</v>
+      <c r="A26" s="1">
+        <v>1512181</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N26" s="1">
+        <v>53797</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>1510072</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N27" s="2">
-        <v>53335</v>
+      <c r="A27" s="1">
+        <v>1512183</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N27" s="1">
+        <v>53655</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>1503101</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N28" s="2">
-        <v>53667</v>
+      <c r="A28" s="1">
+        <v>1512221</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N28" s="1">
+        <v>53954</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>1611281</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N29" s="2">
-        <v>54247</v>
+      <c r="A29" s="1">
+        <v>1601074</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N29" s="1">
+        <v>53457</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>1605022</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N30" s="2">
-        <v>53856</v>
+      <c r="A30" s="1">
+        <v>1601284</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N30" s="1">
+        <v>53591</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>1512221</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N31" s="2">
-        <v>53954</v>
+      <c r="A31" s="1">
+        <v>1602191</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N31" s="1">
+        <v>53899</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>1511181</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N32" s="2">
-        <v>53609</v>
+      <c r="A32" s="1">
+        <v>1603154</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N32" s="1">
+        <v>53641</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>1411184</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D33" s="2">
-        <v>1024</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N33" s="2">
-        <v>53664</v>
+      <c r="A33" s="1">
+        <v>1603156</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N33" s="1">
+        <v>54053</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>1411083</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N34" s="2">
-        <v>53934</v>
+      <c r="A34" s="1">
+        <v>1605022</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N34" s="1">
+        <v>53856</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>1707271</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N35" s="2">
-        <v>54852</v>
+      <c r="A35" s="1">
+        <v>1605115</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N35" s="1">
+        <v>54067</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>1605115</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N36" s="2">
-        <v>54067</v>
+      <c r="A36" s="1">
+        <v>1605163</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N36" s="1">
+        <v>53862</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>1701192</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N37" s="2">
-        <v>54358</v>
+      <c r="A37" s="1">
+        <v>1605183</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N37" s="1">
+        <v>53858</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>1512183</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N38" s="2">
-        <v>53655</v>
+      <c r="A38" s="1">
+        <v>1606061</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N38" s="1">
+        <v>53976</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>1512181</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N39" s="2">
-        <v>53797</v>
+      <c r="A39" s="1">
+        <v>1606164</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N39" s="1">
+        <v>54066</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <v>1512179</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N40" s="2">
-        <v>53416</v>
+      <c r="A40" s="1">
+        <v>1606164</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N40" s="1">
+        <v>54033</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
-        <v>1512178</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N41" s="2">
-        <v>53415</v>
+      <c r="A41" s="1">
+        <v>1606167</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N41" s="1">
+        <v>54032</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
-        <v>1512177</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N42" s="2">
-        <v>53425</v>
+      <c r="A42" s="1">
+        <v>1607112</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N42" s="1">
+        <v>54185</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>1512176</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M43" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N43" s="2">
-        <v>53656</v>
+      <c r="A43" s="1">
+        <v>1607201</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N43" s="1">
+        <v>54087</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <v>1512175</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N44" s="2">
-        <v>53422</v>
+      <c r="A44" s="1">
+        <v>1607222</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N44" s="1">
+        <v>54034</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <v>1607222</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N45" s="2">
-        <v>54034</v>
+      <c r="A45" s="1">
+        <v>1608051</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N45" s="1">
+        <v>54140</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
-        <v>1605183</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N46" s="2">
-        <v>53858</v>
+      <c r="A46" s="1">
+        <v>1608303</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N46" s="1">
+        <v>54162</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
-        <v>1507061</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N47" s="2">
-        <v>53617</v>
+      <c r="A47" s="1">
+        <v>1610041</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N47" s="1">
+        <v>54351</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>1603156</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L48" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M48" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N48" s="2">
-        <v>54053</v>
+      <c r="A48" s="1">
+        <v>1610042</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N48" s="1">
+        <v>54348</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <v>1602191</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N49" s="2">
-        <v>53899</v>
+      <c r="A49" s="1">
+        <v>1610071</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N49" s="1">
+        <v>54190</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
-        <v>1710195</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M50" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N50" s="2">
-        <v>54869</v>
+      <c r="A50" s="1">
+        <v>1611085</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N50" s="1">
+        <v>54705</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
-        <v>1504271</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L51" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M51" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N51" s="2">
-        <v>54020</v>
+      <c r="A51" s="1">
+        <v>1611103</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N51" s="1">
+        <v>54365</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
-        <v>1706012</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L52" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M52" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N52" s="2">
-        <v>54911</v>
+      <c r="A52" s="1">
+        <v>1611281</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N52" s="1">
+        <v>54247</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
-        <v>1606167</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M53" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N53" s="2">
-        <v>54032</v>
+      <c r="A53" s="1">
+        <v>1612271</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N53" s="1">
+        <v>54414</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
-        <v>1510291</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L54" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M54" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N54" s="2">
-        <v>53337</v>
+      <c r="A54" s="1">
+        <v>1701057</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N54" s="1">
+        <v>54521</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
-        <v>1507284</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M55" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N55" s="2">
-        <v>53275</v>
+      <c r="A55" s="1">
+        <v>1701112</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N55" s="1">
+        <v>54418</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
-        <v>1605163</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L56" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M56" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N56" s="2">
-        <v>53862</v>
+      <c r="A56" s="1">
+        <v>1701192</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N56" s="1">
+        <v>54358</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
-        <v>1608051</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="K57" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L57" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M57" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N57" s="2">
-        <v>54140</v>
+      <c r="A57" s="1">
+        <v>1701201</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N57" s="1">
+        <v>54416</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
-        <v>1510094</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M58" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N58" s="2">
-        <v>53525</v>
+      <c r="A58" s="1">
+        <v>1701314</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N58" s="1">
+        <v>54953</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
-        <v>1610071</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="K59" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L59" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M59" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N59" s="2">
-        <v>54190</v>
+      <c r="A59" s="1">
+        <v>1703153</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
-        <v>1504282</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="K60" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L60" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M60" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N60" s="2">
-        <v>53266</v>
+      <c r="A60" s="1">
+        <v>1703271</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N60" s="1">
+        <v>54483</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
-        <v>1507142</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="K61" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L61" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M61" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N61" s="2">
-        <v>53802</v>
+      <c r="A61" s="1">
+        <v>1704031</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H61" s="2"/>
+      <c r="I61" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N61" s="1">
+        <v>54558</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <v>1507094</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K62" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L62" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M62" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N62" s="2">
-        <v>54111</v>
+      <c r="A62" s="1">
+        <v>1705092</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N62" s="1">
+        <v>54711</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>1701314</v>
+        <v>1705111</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C63" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="D63" s="1" t="s">
-        <v>215</v>
+        <v>91</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="K63" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L63" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M63" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M63" s="1" t="s">
         <v>19</v>
       </c>
       <c r="N63" s="1">
-        <v>54953</v>
+        <v>54724</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>1705092</v>
+        <v>1706012</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C64" s="1"/>
+        <v>180</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>181</v>
+      </c>
       <c r="D64" s="1" t="s">
-        <v>217</v>
+        <v>182</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="K64" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L64" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M64" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M64" s="1" t="s">
         <v>19</v>
       </c>
       <c r="N64" s="1">
-        <v>54711</v>
+        <v>54911</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>1710121</v>
+        <v>1706301</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="K65" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L65" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M65" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M65" s="1" t="s">
         <v>19</v>
       </c>
       <c r="N65" s="1">
-        <v>55135</v>
+        <v>55026</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>1607112</v>
+        <v>1707271</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C66" s="1"/>
+        <v>131</v>
+      </c>
       <c r="D66" s="1" t="s">
-        <v>222</v>
+        <v>132</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="K66" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L66" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M66" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M66" s="1" t="s">
         <v>19</v>
       </c>
       <c r="N66" s="1">
-        <v>54185</v>
+        <v>54852</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>1710134</v>
+        <v>1708141</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>180</v>
+        <v>87</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>224</v>
+        <v>88</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>225</v>
+        <v>89</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="K67" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L67" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M67" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M67" s="1" t="s">
         <v>19</v>
       </c>
       <c r="N67" s="1">
-        <v>54990</v>
+        <v>54871</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
@@ -8801,293 +8773,297 @@
       <c r="E68" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="F68" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H68" s="3">
+      <c r="F68" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H68" s="2">
         <v>43187</v>
       </c>
-      <c r="I68" s="2" t="s">
+      <c r="I68" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="J68" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="K68" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L68" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M68" s="2" t="s">
+      <c r="K68" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M68" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>1706301</v>
+        <v>1710121</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C69" s="1"/>
+        <v>172</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="D69" s="1" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="K69" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L69" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M69" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M69" s="1" t="s">
         <v>19</v>
       </c>
       <c r="N69" s="1">
-        <v>55026</v>
+        <v>55135</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>1703153</v>
+        <v>1710133</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>233</v>
+        <v>11</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>234</v>
+        <v>34</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E70" s="1"/>
-      <c r="F70" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J70" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L70" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>1703271</v>
+        <v>1710134</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>238</v>
+        <v>180</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="K71" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L71" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M71" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M71" s="1" t="s">
         <v>19</v>
       </c>
       <c r="N71" s="1">
-        <v>54483</v>
+        <v>54990</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>1801052</v>
+        <v>1710195</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>242</v>
+        <v>172</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>243</v>
+        <v>173</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>243</v>
+        <v>174</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="K72" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M72" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M72" s="1" t="s">
         <v>19</v>
       </c>
       <c r="N72" s="1">
-        <v>55139</v>
+        <v>54869</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>1312171</v>
-      </c>
-      <c r="B73" s="1"/>
+        <v>1711032</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>247</v>
+      </c>
       <c r="C73" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E73" s="1"/>
-      <c r="I73" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I73" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>1711032</v>
+        <v>1712081</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>35</v>
+        <v>254</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>13</v>
+        <v>255</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>1712084</v>
+        <v>1712082</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>252</v>
+        <v>262</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>1712081</v>
+        <v>1712083</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C76" s="1"/>
+        <v>256</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>257</v>
+      </c>
       <c r="D76" s="1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>255</v>
+        <v>259</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>1712083</v>
+        <v>1712084</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>13</v>
+        <v>252</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>1712082</v>
+        <v>1712192</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>260</v>
+        <v>180</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="I78" s="2" t="s">
-        <v>13</v>
+        <v>265</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>1712192</v>
+        <v>1801052</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>180</v>
+        <v>242</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J79" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K79" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L79" s="2" t="s">
-        <v>19</v>
+        <v>244</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L79" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N79" s="1">
+        <v>55139</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
@@ -9097,19 +9073,22 @@
       <c r="B80" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
         <v>266</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="I80" s="2" t="s">
+      <c r="I80" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{4EE4147E-D3AC-4AB4-86BA-051B75939799}"/>
+  <autoFilter ref="A1:N1" xr:uid="{4EE4147E-D3AC-4AB4-86BA-051B75939799}">
+    <sortState ref="A2:N80">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <conditionalFormatting sqref="C2:E2 A23:E26">
     <cfRule type="expression" dxfId="743" priority="745">
       <formula>$G2="Waiting for Check and Letter"</formula>
@@ -11635,4 +11614,119 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F5C25B-7545-47C9-8C29-F7AC4E50DDD8}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5">
+        <v>43117</v>
+      </c>
+      <c r="B1" s="5">
+        <v>43104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>43152</v>
+      </c>
+      <c r="B2" s="5">
+        <v>43139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>43180</v>
+      </c>
+      <c r="B3" s="5">
+        <v>43168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>43208</v>
+      </c>
+      <c r="B4" s="5">
+        <v>43196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>43236</v>
+      </c>
+      <c r="B5" s="5">
+        <v>43224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>43271</v>
+      </c>
+      <c r="B6" s="5">
+        <v>43259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>43299</v>
+      </c>
+      <c r="B7" s="5">
+        <v>43287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>43327</v>
+      </c>
+      <c r="B8" s="5">
+        <v>43315</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>43362</v>
+      </c>
+      <c r="B9" s="5">
+        <v>43350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>43390</v>
+      </c>
+      <c r="B10" s="5">
+        <v>43377</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>43418</v>
+      </c>
+      <c r="B11" s="5">
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>43453</v>
+      </c>
+      <c r="B12" s="5">
+        <v>43441</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished email logic, removed test data, commented out directory location.  Before deploying, set directory to directory location
</commit_message>
<xml_diff>
--- a/AdvisoryBoardTracking.xlsx
+++ b/AdvisoryBoardTracking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john\Desktop\AdvisoryBoardStatusEmailer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John Paradise\MyPythonScripts\AdvisoryBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22EB3DC-0783-4F94-9AEF-8CA404D22B93}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F2B6BE-38A6-44B7-AE1C-1446C0F7F258}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10995" activeTab="2" xr2:uid="{16EC1FD0-7CA3-47E8-B2E3-1D4E6D661775}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10995" activeTab="1" xr2:uid="{16EC1FD0-7CA3-47E8-B2E3-1D4E6D661775}"/>
   </bookViews>
   <sheets>
     <sheet name="NewSubmissions" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NewSubmissions!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PendingReSubmissions!$A$1:$K$1</definedName>
     <definedName name="Engineers">'[1]Drop Down List Info'!$E$1:$E$6</definedName>
     <definedName name="NYCABStatus">'[1]Drop Down List Info'!$A$1:$A$9</definedName>
   </definedNames>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="267">
   <si>
     <t>SO#</t>
   </si>
@@ -85,9 +86,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Harris</t>
-  </si>
-  <si>
     <t>Manhattan West</t>
   </si>
   <si>
@@ -112,15 +110,6 @@
     <t>ZXY</t>
   </si>
   <si>
-    <t>Farts</t>
-  </si>
-  <si>
-    <t>Zippidy</t>
-  </si>
-  <si>
-    <t>dfa</t>
-  </si>
-  <si>
     <t>Billy</t>
   </si>
   <si>
@@ -839,6 +828,15 @@
   </si>
   <si>
     <t>18A0277</t>
+  </si>
+  <si>
+    <t>Original Meeting Submit</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -889,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -904,6 +902,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6814,30 +6813,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EEE128-BC57-4ED5-B88C-215F6AB7547E}">
   <dimension ref="A1:N80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1328125" style="1"/>
+    <col min="2" max="2" width="16.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1328125" style="1"/>
     <col min="6" max="6" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="17.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.1328125" style="1"/>
+    <col min="11" max="11" width="16.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6869,262 +6868,262 @@
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1312171</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1411083</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N3" s="1">
         <v>53934</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>1411184</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D4" s="1">
         <v>1024</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N4" s="1">
         <v>53664</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>1503101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N5" s="1">
         <v>53667</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>1503201</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N6" s="1">
         <v>53439</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>1503201</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N7" s="1">
         <v>53831</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>1504271</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N8" s="1">
         <v>54020</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>1504282</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N9" s="1">
         <v>53266</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>1507061</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="K10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N10" s="1">
         <v>53617</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>1507093</v>
       </c>
@@ -7132,1393 +7131,1393 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="K11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N11" s="1">
         <v>53611</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>1507094</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N12" s="1">
         <v>54111</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>1507142</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N13" s="1">
         <v>53802</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>1507284</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N14" s="1">
         <v>53275</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>1510012</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N15" s="1">
         <v>53438</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>1510022</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N16" s="1">
         <v>53370</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>1510072</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N17" s="1">
         <v>53335</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>1510094</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N18" s="1">
         <v>53525</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>1510291</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N19" s="1">
         <v>53337</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>1511181</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="D20" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N20" s="1">
         <v>53609</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>1512175</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N21" s="1">
         <v>53422</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>1512176</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N22" s="1">
         <v>53656</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>1512177</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N23" s="1">
         <v>53425</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>1512178</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N24" s="1">
         <v>53415</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>1512179</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N25" s="1">
         <v>53416</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>1512181</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="K26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N26" s="1">
         <v>53797</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>1512183</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N27" s="1">
         <v>53655</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>1512221</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N28" s="1">
         <v>53954</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>1601074</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="K29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N29" s="1">
         <v>53457</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>1601284</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N30" s="1">
         <v>53591</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>1602191</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="D31" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N31" s="1">
         <v>53899</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>1603154</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N32" s="1">
         <v>53641</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>1603156</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N33" s="1">
         <v>54053</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>1605022</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="E34" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N34" s="1">
         <v>53856</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>1605115</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N35" s="1">
         <v>54067</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>1605163</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N36" s="1">
         <v>53862</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>1605183</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="E37" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N37" s="1">
         <v>53858</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>1606061</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N38" s="1">
         <v>53976</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>1606164</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N39" s="1">
         <v>54066</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>1606164</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="K40" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N40" s="1">
         <v>54033</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>1606167</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="D41" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N41" s="1">
         <v>54032</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>1607112</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N42" s="1">
         <v>54185</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>1607201</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N43" s="1">
         <v>54087</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>1607222</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N44" s="1">
         <v>54034</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>1608051</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N45" s="1">
         <v>54140</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>1608303</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N46" s="1">
         <v>54162</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>1610041</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="K47" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N47" s="1">
         <v>54351</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>1610042</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N48" s="1">
         <v>54348</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>1610071</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N49" s="1">
         <v>54190</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>1611085</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N50" s="1">
         <v>54705</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>1611103</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N51" s="1">
         <v>54365</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>1611281</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N52" s="1">
         <v>54247</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>1612271</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N53" s="1">
         <v>54414</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>1701057</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N54" s="1">
         <v>54521</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>1701112</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E55" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N55" s="1">
         <v>54418</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>1701192</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N56" s="1">
         <v>54358</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>1701201</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N57" s="1">
         <v>54416</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>1701314</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N58" s="1">
         <v>54953</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>1703153</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>15</v>
@@ -8527,307 +8526,307 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>1703271</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N60" s="1">
         <v>54483</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>1704031</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N61" s="1">
         <v>54558</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>1705092</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N62" s="1">
         <v>54711</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>1705111</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="K63" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N63" s="1">
         <v>54724</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>1706012</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N64" s="1">
         <v>54911</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>1706301</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N65" s="1">
         <v>55026</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>1707271</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N66" s="1">
         <v>54852</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>1708141</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N67" s="1">
         <v>54871</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>1710033</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H68" s="2">
         <v>43187</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>1710121</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N69" s="1">
         <v>55135</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>1710133</v>
       </c>
@@ -8835,91 +8834,91 @@
         <v>11</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>1710134</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N71" s="1">
         <v>54990</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>1710195</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N72" s="1">
         <v>54869</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>1711032</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>12</v>
@@ -8928,156 +8927,156 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>1712081</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>1712082</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="E75" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>1712083</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>1712084</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>1712192</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>1801052</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N79" s="1">
         <v>55139</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>1801302</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>13</v>
@@ -11514,23 +11513,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4336759-1B85-4BCB-B4FE-7D008B816532}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1328125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11553,65 +11553,52 @@
         <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" t="s">
-        <v>21</v>
+      <c r="K1" s="6" t="s">
+        <v>264</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1234546</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2">
-        <v>1234</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>9876545</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>1232</v>
+      </c>
+      <c r="B4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>1231234</v>
+      </c>
+      <c r="B5" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K1" xr:uid="{48FAFD62-9688-4237-B5E2-4C25E0E43923}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11620,17 +11607,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F5C25B-7545-47C9-8C29-F7AC4E50DDD8}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="5">
         <v>43117</v>
       </c>
@@ -11638,7 +11625,7 @@
         <v>43104</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
         <v>43152</v>
       </c>
@@ -11646,7 +11633,7 @@
         <v>43139</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>43180</v>
       </c>
@@ -11654,7 +11641,7 @@
         <v>43168</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>43208</v>
       </c>
@@ -11662,7 +11649,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>43236</v>
       </c>
@@ -11670,7 +11657,7 @@
         <v>43224</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
         <v>43271</v>
       </c>
@@ -11678,7 +11665,7 @@
         <v>43259</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>43299</v>
       </c>
@@ -11686,7 +11673,7 @@
         <v>43287</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>43327</v>
       </c>
@@ -11694,7 +11681,7 @@
         <v>43315</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>43362</v>
       </c>
@@ -11702,7 +11689,7 @@
         <v>43350</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
         <v>43390</v>
       </c>
@@ -11710,7 +11697,7 @@
         <v>43377</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>43418</v>
       </c>
@@ -11718,7 +11705,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="5">
         <v>43453</v>
       </c>

</xml_diff>

<commit_message>
Added back subject, accidentally deleted.  Finalized project except still have testing email.  Comment out testing email on distributed script
</commit_message>
<xml_diff>
--- a/AdvisoryBoardTracking.xlsx
+++ b/AdvisoryBoardTracking.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John Paradise\MyPythonScripts\AdvisoryBoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john\Desktop\AdvisoryBoardStatusEmailer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F2B6BE-38A6-44B7-AE1C-1446C0F7F258}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC880A89-8411-4EF9-BC54-AC7621800ACC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10995" activeTab="1" xr2:uid="{16EC1FD0-7CA3-47E8-B2E3-1D4E6D661775}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="263">
   <si>
     <t>SO#</t>
   </si>
@@ -104,12 +104,6 @@
     <t>All Info Received</t>
   </si>
   <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>ZXY</t>
-  </si>
-  <si>
     <t>Billy</t>
   </si>
   <si>
@@ -831,12 +825,6 @@
   </si>
   <si>
     <t>Original Meeting Submit</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -6819,24 +6807,24 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="1"/>
-    <col min="2" max="2" width="16.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.1328125" style="1"/>
-    <col min="11" max="11" width="16.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.1328125" style="1"/>
+    <col min="8" max="8" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6880,35 +6868,35 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1312171</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1411083</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>18</v>
@@ -6923,21 +6911,21 @@
         <v>53934</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1411184</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D4" s="1">
         <v>1024</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>18</v>
@@ -6952,21 +6940,21 @@
         <v>53664</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1503101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>18</v>
@@ -6981,18 +6969,18 @@
         <v>53667</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1503201</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>18</v>
@@ -7007,21 +6995,21 @@
         <v>53439</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1503201</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>18</v>
@@ -7036,21 +7024,21 @@
         <v>53831</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1504271</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>18</v>
@@ -7065,21 +7053,21 @@
         <v>54020</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1504282</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>18</v>
@@ -7094,21 +7082,21 @@
         <v>53266</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1507061</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>18</v>
@@ -7123,7 +7111,7 @@
         <v>53617</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1507093</v>
       </c>
@@ -7131,19 +7119,19 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>18</v>
@@ -7158,12 +7146,12 @@
         <v>53611</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1507094</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>16</v>
@@ -7184,18 +7172,18 @@
         <v>54111</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1507142</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>18</v>
@@ -7210,21 +7198,21 @@
         <v>53802</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1507284</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>18</v>
@@ -7239,21 +7227,21 @@
         <v>53275</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1510012</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>18</v>
@@ -7268,21 +7256,21 @@
         <v>53438</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1510022</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>18</v>
@@ -7297,21 +7285,21 @@
         <v>53370</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1510072</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>18</v>
@@ -7326,21 +7314,21 @@
         <v>53335</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1510094</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>18</v>
@@ -7355,21 +7343,21 @@
         <v>53525</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1510291</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>18</v>
@@ -7384,21 +7372,21 @@
         <v>53337</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1511181</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>18</v>
@@ -7413,21 +7401,21 @@
         <v>53609</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1512175</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>18</v>
@@ -7442,21 +7430,21 @@
         <v>53422</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1512176</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>18</v>
@@ -7471,21 +7459,21 @@
         <v>53656</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1512177</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>18</v>
@@ -7500,21 +7488,21 @@
         <v>53425</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1512178</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>18</v>
@@ -7529,21 +7517,21 @@
         <v>53415</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1512179</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>18</v>
@@ -7558,21 +7546,21 @@
         <v>53416</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1512181</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>18</v>
@@ -7587,21 +7575,21 @@
         <v>53797</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1512183</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>18</v>
@@ -7616,21 +7604,21 @@
         <v>53655</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1512221</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>18</v>
@@ -7645,21 +7633,21 @@
         <v>53954</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1601074</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>18</v>
@@ -7674,21 +7662,21 @@
         <v>53457</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1601284</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>18</v>
@@ -7703,21 +7691,21 @@
         <v>53591</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1602191</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>18</v>
@@ -7732,21 +7720,21 @@
         <v>53899</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1603154</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>18</v>
@@ -7761,21 +7749,21 @@
         <v>53641</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>1603156</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>18</v>
@@ -7790,18 +7778,18 @@
         <v>54053</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>1605022</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>18</v>
@@ -7816,21 +7804,21 @@
         <v>53856</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1605115</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="E35" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>18</v>
@@ -7845,18 +7833,18 @@
         <v>54067</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1605163</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>18</v>
@@ -7871,21 +7859,21 @@
         <v>53862</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1605183</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>18</v>
@@ -7900,21 +7888,21 @@
         <v>53858</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1606061</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>18</v>
@@ -7929,21 +7917,21 @@
         <v>53976</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>1606164</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>18</v>
@@ -7958,21 +7946,21 @@
         <v>54066</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1606164</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>18</v>
@@ -7987,21 +7975,21 @@
         <v>54033</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>1606167</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>18</v>
@@ -8016,18 +8004,18 @@
         <v>54032</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>1607112</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>18</v>
@@ -8042,21 +8030,21 @@
         <v>54185</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>1607201</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>18</v>
@@ -8071,21 +8059,21 @@
         <v>54087</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>1607222</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>18</v>
@@ -8100,21 +8088,21 @@
         <v>54034</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>1608051</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>18</v>
@@ -8129,21 +8117,21 @@
         <v>54140</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>1608303</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>18</v>
@@ -8158,21 +8146,21 @@
         <v>54162</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>1610041</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>18</v>
@@ -8187,21 +8175,21 @@
         <v>54351</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>1610042</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>18</v>
@@ -8216,21 +8204,21 @@
         <v>54348</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>1610071</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>18</v>
@@ -8245,21 +8233,21 @@
         <v>54190</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>1611085</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>18</v>
@@ -8274,21 +8262,21 @@
         <v>54705</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>1611103</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>18</v>
@@ -8303,21 +8291,21 @@
         <v>54365</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>1611281</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>18</v>
@@ -8332,18 +8320,18 @@
         <v>54247</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>1612271</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>18</v>
@@ -8358,21 +8346,21 @@
         <v>54414</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>1701057</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>18</v>
@@ -8387,18 +8375,18 @@
         <v>54521</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>1701112</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>18</v>
@@ -8413,18 +8401,18 @@
         <v>54418</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>1701192</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>18</v>
@@ -8439,21 +8427,21 @@
         <v>54358</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>1701201</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>18</v>
@@ -8468,18 +8456,18 @@
         <v>54416</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>1701314</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>18</v>
@@ -8494,30 +8482,30 @@
         <v>54953</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>1703153</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>15</v>
@@ -8526,21 +8514,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>1703271</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>18</v>
@@ -8555,25 +8543,25 @@
         <v>54483</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>1704031</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>14</v>
@@ -8591,18 +8579,18 @@
         <v>54558</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>1705092</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>18</v>
@@ -8617,21 +8605,21 @@
         <v>54711</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>1705111</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>18</v>
@@ -8646,21 +8634,21 @@
         <v>54724</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>1706012</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="E64" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>18</v>
@@ -8675,18 +8663,18 @@
         <v>54911</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>1706301</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>18</v>
@@ -8701,18 +8689,18 @@
         <v>55026</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>1707271</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>18</v>
@@ -8727,21 +8715,21 @@
         <v>54852</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>1708141</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>18</v>
@@ -8756,21 +8744,21 @@
         <v>54871</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>1710033</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>18</v>
@@ -8782,10 +8770,10 @@
         <v>43187</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>18</v>
@@ -8797,21 +8785,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>1710121</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>18</v>
@@ -8826,7 +8814,7 @@
         <v>55135</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>1710133</v>
       </c>
@@ -8834,36 +8822,36 @@
         <v>11</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="I70" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>1710134</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>18</v>
@@ -8878,21 +8866,21 @@
         <v>54990</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>1710195</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="E72" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>18</v>
@@ -8907,18 +8895,18 @@
         <v>54869</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>1711032</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>12</v>
@@ -8927,93 +8915,93 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>1712081</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E74" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>251</v>
-      </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>1712082</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>258</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>1712083</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="E76" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>1712084</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="E77" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>248</v>
-      </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>1712192</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="F78" s="1" t="s">
         <v>18</v>
       </c>
@@ -9021,13 +9009,13 @@
         <v>18</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K78" s="1" t="s">
         <v>18</v>
@@ -9036,21 +9024,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>1801052</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>18</v>
@@ -9065,18 +9053,18 @@
         <v>55139</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>1801302</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>13</v>
@@ -11513,24 +11501,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4336759-1B85-4BCB-B4FE-7D008B816532}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.1328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11562,39 +11550,7 @@
         <v>20</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>1234546</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>9876545</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>1232</v>
-      </c>
-      <c r="B4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>1231234</v>
-      </c>
-      <c r="B5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -11611,13 +11567,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5">
         <v>43117</v>
       </c>
@@ -11625,7 +11581,7 @@
         <v>43104</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>43152</v>
       </c>
@@ -11633,7 +11589,7 @@
         <v>43139</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>43180</v>
       </c>
@@ -11641,7 +11597,7 @@
         <v>43168</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>43208</v>
       </c>
@@ -11649,7 +11605,7 @@
         <v>43196</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>43236</v>
       </c>
@@ -11657,7 +11613,7 @@
         <v>43224</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43271</v>
       </c>
@@ -11665,7 +11621,7 @@
         <v>43259</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>43299</v>
       </c>
@@ -11673,7 +11629,7 @@
         <v>43287</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>43327</v>
       </c>
@@ -11681,7 +11637,7 @@
         <v>43315</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>43362</v>
       </c>
@@ -11689,7 +11645,7 @@
         <v>43350</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>43390</v>
       </c>
@@ -11697,7 +11653,7 @@
         <v>43377</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>43418</v>
       </c>
@@ -11705,7 +11661,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>43453</v>
       </c>

</xml_diff>